<commit_message>
2022.01.05 | Hu Wenqiang | Updated Card
</commit_message>
<xml_diff>
--- a/数据结果.xlsx
+++ b/数据结果.xlsx
@@ -432,6 +432,14 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="19" customWidth="1" min="1" max="1"/>
+    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
+    <col width="40" customWidth="1" min="5" max="5"/>
+    <col width="13" customWidth="1" min="6" max="6"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -501,7 +509,6 @@
           <t>归属地</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -524,7 +531,6 @@
           <t>34</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -557,7 +563,6 @@
           <t>26</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
           <t>安徽阜阳</t>
@@ -590,7 +595,6 @@
           <t>27</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -623,7 +627,6 @@
           <t>39</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
           <t>贵州凯里</t>
@@ -656,7 +659,6 @@
           <t>22</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>河南商丘</t>
@@ -689,7 +691,6 @@
           <t>40</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -722,7 +723,6 @@
           <t>6</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -755,7 +755,6 @@
           <t>23</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -788,7 +787,6 @@
           <t>28</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
           <t>安徽铜陵</t>
@@ -821,7 +819,6 @@
           <t>24</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -854,7 +851,6 @@
           <t>26</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -887,7 +883,6 @@
           <t>39</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -920,7 +915,6 @@
           <t>25</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -953,7 +947,6 @@
           <t>27</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
           <t>浙江金华</t>
@@ -986,7 +979,6 @@
           <t>22</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1019,7 +1011,6 @@
           <t>29</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr">
         <is>
           <t>error: 非法号码!</t>
@@ -1052,7 +1043,6 @@
           <t>52</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1085,7 +1075,6 @@
           <t>26</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
           <t>浙江绍兴</t>
@@ -1108,13 +1097,11 @@
           <t>张彬</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
           <t>18</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
           <t>error: 无输入号码!</t>
@@ -1147,7 +1134,6 @@
           <t>29</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
           <t>湖北咸宁</t>
@@ -1180,7 +1166,6 @@
           <t>13</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1213,7 +1198,6 @@
           <t>35</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
           <t>湖北襄阳</t>
@@ -1246,7 +1230,6 @@
           <t>3</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1279,7 +1262,6 @@
           <t>33</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1312,7 +1294,6 @@
           <t>27</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1345,7 +1326,6 @@
           <t>23</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1378,7 +1358,6 @@
           <t>5</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1411,7 +1390,6 @@
           <t>28</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1444,7 +1422,6 @@
           <t>36</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1477,7 +1454,6 @@
           <t>9</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1510,7 +1486,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
           <t>北京北京</t>
@@ -1543,7 +1518,6 @@
           <t>6</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1576,7 +1550,6 @@
           <t>24</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1609,7 +1582,6 @@
           <t>22</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1642,7 +1614,6 @@
           <t>30</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1675,7 +1646,6 @@
           <t>28</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1708,7 +1678,6 @@
           <t>34</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1741,7 +1710,6 @@
           <t>23</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1774,7 +1742,6 @@
           <t>20</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1807,7 +1774,6 @@
           <t>22</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1840,7 +1806,6 @@
           <t>39</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1873,7 +1838,6 @@
           <t>3</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1906,7 +1870,6 @@
           <t>24</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1939,7 +1902,6 @@
           <t>23</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -1972,7 +1934,6 @@
           <t>32</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
           <t>安徽宿州</t>
@@ -2005,7 +1966,6 @@
           <t>62</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2038,7 +1998,6 @@
           <t>32</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2071,7 +2030,6 @@
           <t>22</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2104,7 +2062,6 @@
           <t>20</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2137,7 +2094,6 @@
           <t>29</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2170,7 +2126,6 @@
           <t>23</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2203,7 +2158,6 @@
           <t>6</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2236,7 +2190,6 @@
           <t>34</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2269,7 +2222,6 @@
           <t>39</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2302,7 +2254,6 @@
           <t>26</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2335,7 +2286,6 @@
           <t>17</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2368,7 +2318,6 @@
           <t>26</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2401,7 +2350,6 @@
           <t>39</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2434,7 +2382,6 @@
           <t>48</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2467,7 +2414,6 @@
           <t>60</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2500,7 +2446,6 @@
           <t>20</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr"/>
       <c r="F63" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2533,7 +2478,6 @@
           <t>20</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2566,7 +2510,6 @@
           <t>70</t>
         </is>
       </c>
-      <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2599,7 +2542,6 @@
           <t>26</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2632,7 +2574,6 @@
           <t>9</t>
         </is>
       </c>
-      <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2665,7 +2606,6 @@
           <t>51</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2698,7 +2638,6 @@
           <t>20</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2731,7 +2670,6 @@
           <t>20</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr"/>
       <c r="F70" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2764,7 +2702,6 @@
           <t>34</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2797,7 +2734,6 @@
           <t>26</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2830,7 +2766,6 @@
           <t>22</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2863,7 +2798,6 @@
           <t>7</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr"/>
       <c r="F74" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2896,7 +2830,6 @@
           <t>25</t>
         </is>
       </c>
-      <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2929,7 +2862,6 @@
           <t>37</t>
         </is>
       </c>
-      <c r="E76" t="inlineStr"/>
       <c r="F76" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2962,7 +2894,6 @@
           <t>57</t>
         </is>
       </c>
-      <c r="E77" t="inlineStr"/>
       <c r="F77" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -2995,7 +2926,6 @@
           <t>26</t>
         </is>
       </c>
-      <c r="E78" t="inlineStr"/>
       <c r="F78" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -3028,7 +2958,6 @@
           <t>12</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr"/>
       <c r="F79" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -3061,7 +2990,6 @@
           <t>19</t>
         </is>
       </c>
-      <c r="E80" t="inlineStr"/>
       <c r="F80" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -3094,7 +3022,6 @@
           <t>24</t>
         </is>
       </c>
-      <c r="E81" t="inlineStr"/>
       <c r="F81" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -3127,7 +3054,6 @@
           <t>30</t>
         </is>
       </c>
-      <c r="E82" t="inlineStr"/>
       <c r="F82" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -3160,7 +3086,6 @@
           <t>37</t>
         </is>
       </c>
-      <c r="E83" t="inlineStr"/>
       <c r="F83" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -3193,7 +3118,6 @@
           <t>26</t>
         </is>
       </c>
-      <c r="E84" t="inlineStr"/>
       <c r="F84" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -3226,7 +3150,6 @@
           <t>31</t>
         </is>
       </c>
-      <c r="E85" t="inlineStr"/>
       <c r="F85" t="inlineStr">
         <is>
           <t>吉林吉林</t>
@@ -3259,7 +3182,6 @@
           <t>7</t>
         </is>
       </c>
-      <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -3292,7 +3214,6 @@
           <t>26</t>
         </is>
       </c>
-      <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr">
         <is>
           <t>江苏苏州</t>
@@ -3325,7 +3246,6 @@
           <t>38</t>
         </is>
       </c>
-      <c r="E88" t="inlineStr"/>
       <c r="F88" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -3358,7 +3278,6 @@
           <t>38</t>
         </is>
       </c>
-      <c r="E89" t="inlineStr"/>
       <c r="F89" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -3391,7 +3310,6 @@
           <t>22</t>
         </is>
       </c>
-      <c r="E90" t="inlineStr"/>
       <c r="F90" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -3424,7 +3342,6 @@
           <t>18</t>
         </is>
       </c>
-      <c r="E91" t="inlineStr"/>
       <c r="F91" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -3457,7 +3374,6 @@
           <t>error: 身份证号有误，无法处理年龄!</t>
         </is>
       </c>
-      <c r="E92" t="inlineStr"/>
       <c r="F92" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -3490,7 +3406,6 @@
           <t>28</t>
         </is>
       </c>
-      <c r="E93" t="inlineStr"/>
       <c r="F93" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -3523,7 +3438,6 @@
           <t>32</t>
         </is>
       </c>
-      <c r="E94" t="inlineStr"/>
       <c r="F94" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -3556,7 +3470,6 @@
           <t>19</t>
         </is>
       </c>
-      <c r="E95" t="inlineStr"/>
       <c r="F95" t="inlineStr">
         <is>
           <t>error: 非法号码!</t>
@@ -3589,7 +3502,6 @@
           <t>10</t>
         </is>
       </c>
-      <c r="E96" t="inlineStr"/>
       <c r="F96" t="inlineStr">
         <is>
           <t>error: 非法号码!</t>
@@ -3612,13 +3524,11 @@
           <t>杨丽</t>
         </is>
       </c>
-      <c r="C97" t="inlineStr"/>
       <c r="D97" t="inlineStr">
         <is>
           <t>39</t>
         </is>
       </c>
-      <c r="E97" t="inlineStr"/>
       <c r="F97" t="inlineStr">
         <is>
           <t>error: 无输入号码!</t>
@@ -3651,7 +3561,6 @@
           <t>40</t>
         </is>
       </c>
-      <c r="E98" t="inlineStr"/>
       <c r="F98" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -3684,7 +3593,6 @@
           <t>57</t>
         </is>
       </c>
-      <c r="E99" t="inlineStr"/>
       <c r="F99" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -3717,7 +3625,6 @@
           <t>26</t>
         </is>
       </c>
-      <c r="E100" t="inlineStr"/>
       <c r="F100" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -3750,7 +3657,6 @@
           <t>27</t>
         </is>
       </c>
-      <c r="E101" t="inlineStr"/>
       <c r="F101" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -3783,7 +3689,6 @@
           <t>error: 身份证号有误，无法处理年龄!</t>
         </is>
       </c>
-      <c r="E102" t="inlineStr"/>
       <c r="F102" t="inlineStr">
         <is>
           <t>浙江杭州</t>
@@ -3796,15 +3701,11 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="inlineStr"/>
-      <c r="B103" t="inlineStr"/>
-      <c r="C103" t="inlineStr"/>
       <c r="D103" t="inlineStr">
         <is>
           <t>error: 身份证号有误，无法处理年龄!</t>
         </is>
       </c>
-      <c r="E103" t="inlineStr"/>
       <c r="F103" t="inlineStr">
         <is>
           <t>error: 无输入号码!</t>

</xml_diff>

<commit_message>
2022.01.05 | Hu Wenqiang | Backup as T1 & T2 Completed
</commit_message>
<xml_diff>
--- a/数据结果.xlsx
+++ b/数据结果.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G103"/>
+  <dimension ref="A1:F103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,11 +472,6 @@
           <t>归属地</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>户籍地址</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -531,14 +526,14 @@
           <t>34</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>湖北省鄂西土家族苗族自治州宣恩县</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>湖北省鄂西土家族苗族自治州宣恩县</t>
         </is>
       </c>
     </row>
@@ -563,14 +558,14 @@
           <t>26</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>辽宁省朝阳市北票市</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
           <t>安徽阜阳</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>辽宁省朝阳市北票市</t>
         </is>
       </c>
     </row>
@@ -595,14 +590,14 @@
           <t>27</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>江苏省淮阴市金湖县</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>江苏省淮阴市金湖县</t>
         </is>
       </c>
     </row>
@@ -627,14 +622,14 @@
           <t>39</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>黑龙江省佳木斯市东风区</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>贵州凯里</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>黑龙江省佳木斯市东风区</t>
         </is>
       </c>
     </row>
@@ -659,14 +654,14 @@
           <t>22</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>江西省上饶市余干县</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>河南商丘</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>江西省上饶市余干县</t>
         </is>
       </c>
     </row>
@@ -691,14 +686,14 @@
           <t>40</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>河南省焦作市焦作市</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>河南省焦作市焦作市</t>
         </is>
       </c>
     </row>
@@ -723,14 +718,14 @@
           <t>6</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>上海市市辖区崇明区</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>上海市市辖区崇明区</t>
         </is>
       </c>
     </row>
@@ -755,14 +750,14 @@
           <t>23</t>
         </is>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>山西省晋中市祁县</t>
+        </is>
+      </c>
       <c r="F10" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>山西省晋中市祁县</t>
         </is>
       </c>
     </row>
@@ -787,14 +782,14 @@
           <t>28</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>河北省保定市定兴县</t>
+        </is>
+      </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>安徽铜陵</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>河北省保定市定兴县</t>
         </is>
       </c>
     </row>
@@ -819,14 +814,14 @@
           <t>24</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>湖北省咸宁市崇阳县</t>
+        </is>
+      </c>
       <c r="F12" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>湖北省咸宁市崇阳县</t>
         </is>
       </c>
     </row>
@@ -851,14 +846,14 @@
           <t>26</t>
         </is>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>四川省宜宾市珙县</t>
+        </is>
+      </c>
       <c r="F13" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>四川省宜宾市珙县</t>
         </is>
       </c>
     </row>
@@ -883,14 +878,14 @@
           <t>39</t>
         </is>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>河北省秦皇岛市海港区</t>
+        </is>
+      </c>
       <c r="F14" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>河北省秦皇岛市海港区</t>
         </is>
       </c>
     </row>
@@ -915,14 +910,14 @@
           <t>25</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>广西壮族自治区玉林市兴业县</t>
+        </is>
+      </c>
       <c r="F15" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>广西壮族自治区玉林市兴业县</t>
         </is>
       </c>
     </row>
@@ -947,14 +942,14 @@
           <t>27</t>
         </is>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>吉林省白城市洮南市</t>
+        </is>
+      </c>
       <c r="F16" t="inlineStr">
         <is>
           <t>浙江金华</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>吉林省白城市洮南市</t>
         </is>
       </c>
     </row>
@@ -979,14 +974,14 @@
           <t>22</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>江西省宜春市宜春市</t>
+        </is>
+      </c>
       <c r="F17" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>江西省宜春市宜春市</t>
         </is>
       </c>
     </row>
@@ -1011,14 +1006,14 @@
           <t>29</t>
         </is>
       </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>四川省南充市仪陇县</t>
+        </is>
+      </c>
       <c r="F18" t="inlineStr">
         <is>
           <t>error: 非法号码!</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>四川省南充市仪陇县</t>
         </is>
       </c>
     </row>
@@ -1043,14 +1038,14 @@
           <t>52</t>
         </is>
       </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>辽宁省锦州市黑山县</t>
+        </is>
+      </c>
       <c r="F19" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>辽宁省锦州市黑山县</t>
         </is>
       </c>
     </row>
@@ -1075,14 +1070,14 @@
           <t>26</t>
         </is>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>湖南省岳阳市岳阳楼区</t>
+        </is>
+      </c>
       <c r="F20" t="inlineStr">
         <is>
           <t>浙江绍兴</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>湖南省岳阳市岳阳楼区</t>
         </is>
       </c>
     </row>
@@ -1102,14 +1097,14 @@
           <t>18</t>
         </is>
       </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>甘肃省天水市秦州区</t>
+        </is>
+      </c>
       <c r="F21" t="inlineStr">
         <is>
           <t>error: 无输入号码!</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>甘肃省天水市秦州区</t>
         </is>
       </c>
     </row>
@@ -1134,14 +1129,14 @@
           <t>29</t>
         </is>
       </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>河北省邢台市新河县</t>
+        </is>
+      </c>
       <c r="F22" t="inlineStr">
         <is>
           <t>湖北咸宁</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>河北省邢台市新河县</t>
         </is>
       </c>
     </row>
@@ -1166,14 +1161,14 @@
           <t>13</t>
         </is>
       </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>江苏省南通市通州区</t>
+        </is>
+      </c>
       <c r="F23" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>江苏省南通市通州区</t>
         </is>
       </c>
     </row>
@@ -1198,14 +1193,14 @@
           <t>35</t>
         </is>
       </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>湖北省鄂州市梁子湖区</t>
+        </is>
+      </c>
       <c r="F24" t="inlineStr">
         <is>
           <t>湖北襄阳</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>湖北省鄂州市梁子湖区</t>
         </is>
       </c>
     </row>
@@ -1230,14 +1225,14 @@
           <t>3</t>
         </is>
       </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>山西省晋中市太谷区</t>
+        </is>
+      </c>
       <c r="F25" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>山西省晋中市太谷区</t>
         </is>
       </c>
     </row>
@@ -1262,14 +1257,14 @@
           <t>33</t>
         </is>
       </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>河南省新乡市新乡县</t>
+        </is>
+      </c>
       <c r="F26" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>河南省新乡市新乡县</t>
         </is>
       </c>
     </row>
@@ -1294,14 +1289,14 @@
           <t>27</t>
         </is>
       </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>河北省邢台市沙河市</t>
+        </is>
+      </c>
       <c r="F27" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>河北省邢台市沙河市</t>
         </is>
       </c>
     </row>
@@ -1326,14 +1321,14 @@
           <t>23</t>
         </is>
       </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>湖南省娄底市娄星区</t>
+        </is>
+      </c>
       <c r="F28" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>湖南省娄底市娄星区</t>
         </is>
       </c>
     </row>
@@ -1358,14 +1353,14 @@
           <t>5</t>
         </is>
       </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>贵州省六盘水市盘州市</t>
+        </is>
+      </c>
       <c r="F29" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>贵州省六盘水市盘州市</t>
         </is>
       </c>
     </row>
@@ -1390,14 +1385,14 @@
           <t>28</t>
         </is>
       </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>山东省德州市齐河县</t>
+        </is>
+      </c>
       <c r="F30" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>山东省德州市齐河县</t>
         </is>
       </c>
     </row>
@@ -1422,14 +1417,14 @@
           <t>36</t>
         </is>
       </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>河北省秦皇岛市青龙满族自治县</t>
+        </is>
+      </c>
       <c r="F31" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>河北省秦皇岛市青龙满族自治县</t>
         </is>
       </c>
     </row>
@@ -1454,14 +1449,14 @@
           <t>9</t>
         </is>
       </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>江苏省南京市高淳区</t>
+        </is>
+      </c>
       <c r="F32" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>江苏省南京市高淳区</t>
         </is>
       </c>
     </row>
@@ -1486,14 +1481,14 @@
           <t>4</t>
         </is>
       </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>山西省长治市上党区</t>
+        </is>
+      </c>
       <c r="F33" t="inlineStr">
         <is>
           <t>北京北京</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>山西省长治市上党区</t>
         </is>
       </c>
     </row>
@@ -1518,14 +1513,14 @@
           <t>6</t>
         </is>
       </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>辽宁省盘锦市大洼区</t>
+        </is>
+      </c>
       <c r="F34" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>辽宁省盘锦市大洼区</t>
         </is>
       </c>
     </row>
@@ -1550,14 +1545,14 @@
           <t>24</t>
         </is>
       </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>贵州省遵义市道真仡佬族苗族自治县</t>
+        </is>
+      </c>
       <c r="F35" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>贵州省遵义市道真仡佬族苗族自治县</t>
         </is>
       </c>
     </row>
@@ -1582,14 +1577,14 @@
           <t>22</t>
         </is>
       </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>山东省菏泽市曹县</t>
+        </is>
+      </c>
       <c r="F36" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>山东省菏泽市曹县</t>
         </is>
       </c>
     </row>
@@ -1614,14 +1609,14 @@
           <t>30</t>
         </is>
       </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>广东省清远市清城区</t>
+        </is>
+      </c>
       <c r="F37" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>广东省清远市清城区</t>
         </is>
       </c>
     </row>
@@ -1646,14 +1641,14 @@
           <t>28</t>
         </is>
       </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>浙江省台州市三门县</t>
+        </is>
+      </c>
       <c r="F38" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>浙江省台州市三门县</t>
         </is>
       </c>
     </row>
@@ -1678,14 +1673,14 @@
           <t>34</t>
         </is>
       </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>天津市市辖区河东区</t>
+        </is>
+      </c>
       <c r="F39" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>天津市市辖区河东区</t>
         </is>
       </c>
     </row>
@@ -1710,14 +1705,14 @@
           <t>23</t>
         </is>
       </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>甘肃省甘南藏族自治州玛曲县</t>
+        </is>
+      </c>
       <c r="F40" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>甘肃省甘南藏族自治州玛曲县</t>
         </is>
       </c>
     </row>
@@ -1742,14 +1737,14 @@
           <t>20</t>
         </is>
       </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>云南省丽江市永胜县</t>
+        </is>
+      </c>
       <c r="F41" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>云南省丽江市永胜县</t>
         </is>
       </c>
     </row>
@@ -1774,14 +1769,14 @@
           <t>22</t>
         </is>
       </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>山西省临汾市乡宁县</t>
+        </is>
+      </c>
       <c r="F42" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>山西省临汾市乡宁县</t>
         </is>
       </c>
     </row>
@@ -1806,14 +1801,14 @@
           <t>39</t>
         </is>
       </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>贵州省黔东南苗族侗族自治州天柱县</t>
+        </is>
+      </c>
       <c r="F43" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>贵州省黔东南苗族侗族自治州天柱县</t>
         </is>
       </c>
     </row>
@@ -1838,14 +1833,14 @@
           <t>3</t>
         </is>
       </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>云南省玉溪市澄江市</t>
+        </is>
+      </c>
       <c r="F44" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>云南省玉溪市澄江市</t>
         </is>
       </c>
     </row>
@@ -1870,14 +1865,14 @@
           <t>24</t>
         </is>
       </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>陕西省宝鸡市渭滨区</t>
+        </is>
+      </c>
       <c r="F45" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>陕西省宝鸡市渭滨区</t>
         </is>
       </c>
     </row>
@@ -1902,14 +1897,14 @@
           <t>23</t>
         </is>
       </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>四川省阿坝藏族羌族自治州金川县</t>
+        </is>
+      </c>
       <c r="F46" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>四川省阿坝藏族羌族自治州金川县</t>
         </is>
       </c>
     </row>
@@ -1934,14 +1929,14 @@
           <t>32</t>
         </is>
       </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>湖南省湘西土家族苗族自治州花垣县</t>
+        </is>
+      </c>
       <c r="F47" t="inlineStr">
         <is>
           <t>安徽宿州</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>湖南省湘西土家族苗族自治州花垣县</t>
         </is>
       </c>
     </row>
@@ -1966,14 +1961,14 @@
           <t>62</t>
         </is>
       </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>内蒙古自治区呼和浩特市托克托县</t>
+        </is>
+      </c>
       <c r="F48" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>内蒙古自治区呼和浩特市托克托县</t>
         </is>
       </c>
     </row>
@@ -1998,14 +1993,14 @@
           <t>32</t>
         </is>
       </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>广东省深圳市罗湖区</t>
+        </is>
+      </c>
       <c r="F49" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>广东省深圳市罗湖区</t>
         </is>
       </c>
     </row>
@@ -2030,14 +2025,14 @@
           <t>22</t>
         </is>
       </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>江西省吉安市泰和县</t>
+        </is>
+      </c>
       <c r="F50" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>江西省吉安市泰和县</t>
         </is>
       </c>
     </row>
@@ -2062,14 +2057,14 @@
           <t>20</t>
         </is>
       </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>甘肃省张掖市高台县</t>
+        </is>
+      </c>
       <c r="F51" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>甘肃省张掖市高台县</t>
         </is>
       </c>
     </row>
@@ -2094,14 +2089,14 @@
           <t>29</t>
         </is>
       </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>湖北省孝感市云梦县</t>
+        </is>
+      </c>
       <c r="F52" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>湖北省孝感市云梦县</t>
         </is>
       </c>
     </row>
@@ -2126,14 +2121,14 @@
           <t>23</t>
         </is>
       </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>黑龙江省绥化市庆安县</t>
+        </is>
+      </c>
       <c r="F53" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>黑龙江省绥化市庆安县</t>
         </is>
       </c>
     </row>
@@ -2158,14 +2153,14 @@
           <t>6</t>
         </is>
       </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>河北省邯郸市肥乡区</t>
+        </is>
+      </c>
       <c r="F54" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>河北省邯郸市肥乡区</t>
         </is>
       </c>
     </row>
@@ -2190,14 +2185,14 @@
           <t>34</t>
         </is>
       </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>广东省惠州市博罗县</t>
+        </is>
+      </c>
       <c r="F55" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>广东省惠州市博罗县</t>
         </is>
       </c>
     </row>
@@ -2222,14 +2217,14 @@
           <t>39</t>
         </is>
       </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>内蒙古自治区赤峰市喀喇沁旗</t>
+        </is>
+      </c>
       <c r="F56" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>内蒙古自治区赤峰市喀喇沁旗</t>
         </is>
       </c>
     </row>
@@ -2254,14 +2249,14 @@
           <t>26</t>
         </is>
       </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>陕西省汉中市汉中市</t>
+        </is>
+      </c>
       <c r="F57" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>陕西省汉中市汉中市</t>
         </is>
       </c>
     </row>
@@ -2286,14 +2281,14 @@
           <t>17</t>
         </is>
       </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>安徽省安庆市宜秀区</t>
+        </is>
+      </c>
       <c r="F58" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>安徽省安庆市宜秀区</t>
         </is>
       </c>
     </row>
@@ -2318,14 +2313,14 @@
           <t>26</t>
         </is>
       </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>陕西省延安市宜川县</t>
+        </is>
+      </c>
       <c r="F59" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>陕西省延安市宜川县</t>
         </is>
       </c>
     </row>
@@ -2350,14 +2345,14 @@
           <t>39</t>
         </is>
       </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>河南省平顶山市鲁山县</t>
+        </is>
+      </c>
       <c r="F60" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>河南省平顶山市鲁山县</t>
         </is>
       </c>
     </row>
@@ -2382,14 +2377,14 @@
           <t>48</t>
         </is>
       </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>山东省济南市天桥区</t>
+        </is>
+      </c>
       <c r="F61" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>山东省济南市天桥区</t>
         </is>
       </c>
     </row>
@@ -2414,14 +2409,14 @@
           <t>60</t>
         </is>
       </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>甘肃省兰州市七里河区</t>
+        </is>
+      </c>
       <c r="F62" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>甘肃省兰州市七里河区</t>
         </is>
       </c>
     </row>
@@ -2446,14 +2441,14 @@
           <t>20</t>
         </is>
       </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>海南省海口市秀英区</t>
+        </is>
+      </c>
       <c r="F63" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>海南省海口市秀英区</t>
         </is>
       </c>
     </row>
@@ -2478,14 +2473,14 @@
           <t>20</t>
         </is>
       </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>甘肃省酒泉市金塔县</t>
+        </is>
+      </c>
       <c r="F64" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>甘肃省酒泉市金塔县</t>
         </is>
       </c>
     </row>
@@ -2510,14 +2505,14 @@
           <t>70</t>
         </is>
       </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>新疆维吾尔自治区喀什地区麦盖提县</t>
+        </is>
+      </c>
       <c r="F65" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>新疆维吾尔自治区喀什地区麦盖提县</t>
         </is>
       </c>
     </row>
@@ -2542,14 +2537,14 @@
           <t>26</t>
         </is>
       </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>河北省沧州市东光县</t>
+        </is>
+      </c>
       <c r="F66" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>河北省沧州市东光县</t>
         </is>
       </c>
     </row>
@@ -2574,14 +2569,14 @@
           <t>9</t>
         </is>
       </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>青海省海东市互助土族自治县</t>
+        </is>
+      </c>
       <c r="F67" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>青海省海东市互助土族自治县</t>
         </is>
       </c>
     </row>
@@ -2606,14 +2601,14 @@
           <t>51</t>
         </is>
       </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>山西省山西省山西省</t>
+        </is>
+      </c>
       <c r="F68" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>山西省山西省山西省</t>
         </is>
       </c>
     </row>
@@ -2638,14 +2633,14 @@
           <t>20</t>
         </is>
       </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>广西壮族自治区崇左市江州区</t>
+        </is>
+      </c>
       <c r="F69" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>广西壮族自治区崇左市江州区</t>
         </is>
       </c>
     </row>
@@ -2670,14 +2665,14 @@
           <t>20</t>
         </is>
       </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>宁夏回族自治区银川市西夏区</t>
+        </is>
+      </c>
       <c r="F70" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>宁夏回族自治区银川市西夏区</t>
         </is>
       </c>
     </row>
@@ -2702,14 +2697,14 @@
           <t>34</t>
         </is>
       </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>广东省肇庆市广宁县</t>
+        </is>
+      </c>
       <c r="F71" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>广东省肇庆市广宁县</t>
         </is>
       </c>
     </row>
@@ -2734,14 +2729,14 @@
           <t>26</t>
         </is>
       </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>陕西省延安市甘泉县</t>
+        </is>
+      </c>
       <c r="F72" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>陕西省延安市甘泉县</t>
         </is>
       </c>
     </row>
@@ -2766,14 +2761,14 @@
           <t>22</t>
         </is>
       </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>江西省吉安市遂川县</t>
+        </is>
+      </c>
       <c r="F73" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>江西省吉安市遂川县</t>
         </is>
       </c>
     </row>
@@ -2798,14 +2793,14 @@
           <t>7</t>
         </is>
       </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>江西省上饶市广丰区</t>
+        </is>
+      </c>
       <c r="F74" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>江西省上饶市广丰区</t>
         </is>
       </c>
     </row>
@@ -2830,14 +2825,14 @@
           <t>25</t>
         </is>
       </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>山东省青岛市莱西市</t>
+        </is>
+      </c>
       <c r="F75" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>山东省青岛市莱西市</t>
         </is>
       </c>
     </row>
@@ -2862,14 +2857,14 @@
           <t>37</t>
         </is>
       </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>福建省漳州市华安县</t>
+        </is>
+      </c>
       <c r="F76" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>福建省漳州市华安县</t>
         </is>
       </c>
     </row>
@@ -2894,14 +2889,14 @@
           <t>57</t>
         </is>
       </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>青海省果洛藏族自治州班玛县</t>
+        </is>
+      </c>
       <c r="F77" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>青海省果洛藏族自治州班玛县</t>
         </is>
       </c>
     </row>
@@ -2926,14 +2921,14 @@
           <t>26</t>
         </is>
       </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>江苏省无锡市宜兴市</t>
+        </is>
+      </c>
       <c r="F78" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>江苏省无锡市宜兴市</t>
         </is>
       </c>
     </row>
@@ -2958,14 +2953,14 @@
           <t>12</t>
         </is>
       </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>云南省文山壮族苗族自治州文山市</t>
+        </is>
+      </c>
       <c r="F79" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>云南省文山壮族苗族自治州文山市</t>
         </is>
       </c>
     </row>
@@ -2990,14 +2985,14 @@
           <t>19</t>
         </is>
       </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>内蒙古自治区巴彦淖尔市乌拉特后旗</t>
+        </is>
+      </c>
       <c r="F80" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>内蒙古自治区巴彦淖尔市乌拉特后旗</t>
         </is>
       </c>
     </row>
@@ -3022,14 +3017,14 @@
           <t>24</t>
         </is>
       </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>河南省信阳市信阳市</t>
+        </is>
+      </c>
       <c r="F81" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>河南省信阳市信阳市</t>
         </is>
       </c>
     </row>
@@ -3054,14 +3049,14 @@
           <t>30</t>
         </is>
       </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>安徽省滁州市琅琊区</t>
+        </is>
+      </c>
       <c r="F82" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>安徽省滁州市琅琊区</t>
         </is>
       </c>
     </row>
@@ -3086,14 +3081,14 @@
           <t>37</t>
         </is>
       </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>新疆维吾尔自治区喀什地区英吉沙县</t>
+        </is>
+      </c>
       <c r="F83" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>新疆维吾尔自治区喀什地区英吉沙县</t>
         </is>
       </c>
     </row>
@@ -3118,14 +3113,14 @@
           <t>26</t>
         </is>
       </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>福建省龙岩市龙岩市</t>
+        </is>
+      </c>
       <c r="F84" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>福建省龙岩市龙岩市</t>
         </is>
       </c>
     </row>
@@ -3150,14 +3145,14 @@
           <t>31</t>
         </is>
       </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>黑龙江省哈尔滨市依兰县</t>
+        </is>
+      </c>
       <c r="F85" t="inlineStr">
         <is>
           <t>吉林吉林</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>黑龙江省哈尔滨市依兰县</t>
         </is>
       </c>
     </row>
@@ -3182,14 +3177,14 @@
           <t>7</t>
         </is>
       </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>陕西省榆林市横山区</t>
+        </is>
+      </c>
       <c r="F86" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>陕西省榆林市横山区</t>
         </is>
       </c>
     </row>
@@ -3214,14 +3209,14 @@
           <t>26</t>
         </is>
       </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>黑龙江省哈尔滨市尚志市</t>
+        </is>
+      </c>
       <c r="F87" t="inlineStr">
         <is>
           <t>江苏苏州</t>
-        </is>
-      </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>黑龙江省哈尔滨市尚志市</t>
         </is>
       </c>
     </row>
@@ -3246,14 +3241,14 @@
           <t>38</t>
         </is>
       </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>青海省玉树藏族自治州称多县</t>
+        </is>
+      </c>
       <c r="F88" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>青海省玉树藏族自治州称多县</t>
         </is>
       </c>
     </row>
@@ -3278,14 +3273,14 @@
           <t>38</t>
         </is>
       </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>湖南省衡阳市衡山县</t>
+        </is>
+      </c>
       <c r="F89" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>湖南省衡阳市衡山县</t>
         </is>
       </c>
     </row>
@@ -3310,14 +3305,14 @@
           <t>22</t>
         </is>
       </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>广东省广州市花都区</t>
+        </is>
+      </c>
       <c r="F90" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>广东省广州市花都区</t>
         </is>
       </c>
     </row>
@@ -3342,14 +3337,14 @@
           <t>18</t>
         </is>
       </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>广西壮族自治区南宁市良庆区</t>
+        </is>
+      </c>
       <c r="F91" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>广西壮族自治区南宁市良庆区</t>
         </is>
       </c>
     </row>
@@ -3374,14 +3369,14 @@
           <t>error: 身份证号有误，无法处理年龄!</t>
         </is>
       </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>error: 身份证号有误，无法处理户籍地址!</t>
+        </is>
+      </c>
       <c r="F92" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>error: 身份证号有误，无法处理户籍地址!</t>
         </is>
       </c>
     </row>
@@ -3406,14 +3401,14 @@
           <t>28</t>
         </is>
       </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>山东省烟台市莱山区</t>
+        </is>
+      </c>
       <c r="F93" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>山东省烟台市莱山区</t>
         </is>
       </c>
     </row>
@@ -3438,14 +3433,14 @@
           <t>32</t>
         </is>
       </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>上海市市辖区徐汇区</t>
+        </is>
+      </c>
       <c r="F94" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>上海市市辖区徐汇区</t>
         </is>
       </c>
     </row>
@@ -3470,14 +3465,14 @@
           <t>19</t>
         </is>
       </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>陕西省宝鸡市陈仓区</t>
+        </is>
+      </c>
       <c r="F95" t="inlineStr">
         <is>
           <t>error: 非法号码!</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>陕西省宝鸡市陈仓区</t>
         </is>
       </c>
     </row>
@@ -3502,14 +3497,14 @@
           <t>10</t>
         </is>
       </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>新疆维吾尔自治区自治区直辖县级行政单位铁门关市</t>
+        </is>
+      </c>
       <c r="F96" t="inlineStr">
         <is>
           <t>error: 非法号码!</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>新疆维吾尔自治区自治区直辖县级行政单位铁门关市</t>
         </is>
       </c>
     </row>
@@ -3529,14 +3524,14 @@
           <t>39</t>
         </is>
       </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>云南省昆明市宜良县</t>
+        </is>
+      </c>
       <c r="F97" t="inlineStr">
         <is>
           <t>error: 无输入号码!</t>
-        </is>
-      </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>云南省昆明市宜良县</t>
         </is>
       </c>
     </row>
@@ -3561,14 +3556,14 @@
           <t>40</t>
         </is>
       </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>黑龙江省大庆市红岗区</t>
+        </is>
+      </c>
       <c r="F98" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>黑龙江省大庆市红岗区</t>
         </is>
       </c>
     </row>
@@ -3593,14 +3588,14 @@
           <t>57</t>
         </is>
       </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>广东省湛江市湛江市</t>
+        </is>
+      </c>
       <c r="F99" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>广东省湛江市湛江市</t>
         </is>
       </c>
     </row>
@@ -3625,14 +3620,14 @@
           <t>26</t>
         </is>
       </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>江苏省宿迁市宿迁市</t>
+        </is>
+      </c>
       <c r="F100" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>江苏省宿迁市宿迁市</t>
         </is>
       </c>
     </row>
@@ -3657,14 +3652,14 @@
           <t>27</t>
         </is>
       </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>辽宁省铁岭市开原市</t>
+        </is>
+      </c>
       <c r="F101" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>辽宁省铁岭市开原市</t>
         </is>
       </c>
     </row>
@@ -3689,14 +3684,14 @@
           <t>error: 身份证号有误，无法处理年龄!</t>
         </is>
       </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>error: 身份证号有误，无法处理户籍地址!</t>
+        </is>
+      </c>
       <c r="F102" t="inlineStr">
         <is>
           <t>浙江杭州</t>
-        </is>
-      </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>error: 身份证号有误，无法处理户籍地址!</t>
         </is>
       </c>
     </row>
@@ -3706,14 +3701,14 @@
           <t>error: 身份证号有误，无法处理年龄!</t>
         </is>
       </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>error: 身份证号有误，无法处理户籍地址!</t>
+        </is>
+      </c>
       <c r="F103" t="inlineStr">
         <is>
           <t>error: 无输入号码!</t>
-        </is>
-      </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>error: 身份证号有误，无法处理户籍地址!</t>
         </is>
       </c>
     </row>

</xml_diff>